<commit_message>
title and events cap
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">important</t>
   </si>
   <si>
-    <t xml:space="preserve">19. 08. 2025</t>
+    <t xml:space="preserve">20. 08. 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Nedělní setkání</t>
@@ -61,9 +61,6 @@
     <t xml:space="preserve">x</t>
   </si>
   <si>
-    <t xml:space="preserve">20. 08. 2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vaječina</t>
   </si>
   <si>
@@ -97,7 +94,7 @@
     <t xml:space="preserve">21.8.2025</t>
   </si>
   <si>
-    <t xml:space="preserve">přednáška na náměstí</t>
+    <t xml:space="preserve">Přednáška na náměstí</t>
   </si>
   <si>
     <t xml:space="preserve">náměstí</t>
@@ -130,7 +127,7 @@
     <t xml:space="preserve">20.8.2027</t>
   </si>
   <si>
-    <t xml:space="preserve">pečení</t>
+    <t xml:space="preserve">Pečení</t>
   </si>
   <si>
     <t xml:space="preserve">Β</t>
@@ -321,7 +318,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -451,7 +448,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -501,7 +498,7 @@
       <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -510,22 +507,22 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>0.583333333333333</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>12</v>
@@ -533,28 +530,28 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>0.666666666666667</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>0.53125</v>
@@ -563,22 +560,22 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>0.333333333333333</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>12</v>
@@ -586,7 +583,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -598,9 +595,9 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -609,156 +606,156 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>1.53125</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>2.53125</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="G9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="0" t="s">
+      <c r="H9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>3.53125</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>4.53125</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>5.53125</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="G12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="0" t="s">
+      <c r="H12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>6.53125</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>7.53125</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="G14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="H14" s="0" t="s">
+      <c r="H14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>8.53125</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>